<commit_message>
added updated gantt chart
</commit_message>
<xml_diff>
--- a/docs/general/project/499_GanttChart.xlsx
+++ b/docs/general/project/499_GanttChart.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25930"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4430359-34AF-4144-9959-5A9626A03A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{39E5ED6A-8A93-4039-ADDB-C48479336AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <definedName name="task_start" localSheetId="0">ProjectSchedule!$E1</definedName>
     <definedName name="today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -205,7 +205,10 @@
     <t>Report - User Groups &amp; Tasks</t>
   </si>
   <si>
-    <t>Report- Issues Discovered</t>
+    <t>Report - Participant Information</t>
+  </si>
+  <si>
+    <t>Report - Issues Discovered</t>
   </si>
   <si>
     <t>Report - Bar Graph of Scores</t>
@@ -1407,11 +1410,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL43"/>
+  <dimension ref="A1:BL44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="101" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -1472,11 +1475,11 @@
       </c>
       <c r="D4" s="84"/>
       <c r="E4" s="7">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I4" s="80">
         <f>I5</f>
-        <v>44858</v>
+        <v>44900</v>
       </c>
       <c r="J4" s="81"/>
       <c r="K4" s="81"/>
@@ -1486,7 +1489,7 @@
       <c r="O4" s="82"/>
       <c r="P4" s="80">
         <f>P5</f>
-        <v>44865</v>
+        <v>44907</v>
       </c>
       <c r="Q4" s="81"/>
       <c r="R4" s="81"/>
@@ -1496,7 +1499,7 @@
       <c r="V4" s="82"/>
       <c r="W4" s="80">
         <f>W5</f>
-        <v>44872</v>
+        <v>44914</v>
       </c>
       <c r="X4" s="81"/>
       <c r="Y4" s="81"/>
@@ -1506,7 +1509,7 @@
       <c r="AC4" s="82"/>
       <c r="AD4" s="80">
         <f>AD5</f>
-        <v>44879</v>
+        <v>44921</v>
       </c>
       <c r="AE4" s="81"/>
       <c r="AF4" s="81"/>
@@ -1516,7 +1519,7 @@
       <c r="AJ4" s="82"/>
       <c r="AK4" s="80">
         <f>AK5</f>
-        <v>44886</v>
+        <v>44928</v>
       </c>
       <c r="AL4" s="81"/>
       <c r="AM4" s="81"/>
@@ -1526,7 +1529,7 @@
       <c r="AQ4" s="82"/>
       <c r="AR4" s="80">
         <f>AR5</f>
-        <v>44893</v>
+        <v>44935</v>
       </c>
       <c r="AS4" s="81"/>
       <c r="AT4" s="81"/>
@@ -1536,7 +1539,7 @@
       <c r="AX4" s="82"/>
       <c r="AY4" s="80">
         <f>AY5</f>
-        <v>44900</v>
+        <v>44942</v>
       </c>
       <c r="AZ4" s="81"/>
       <c r="BA4" s="81"/>
@@ -1546,7 +1549,7 @@
       <c r="BE4" s="82"/>
       <c r="BF4" s="80">
         <f>BF5</f>
-        <v>44907</v>
+        <v>44949</v>
       </c>
       <c r="BG4" s="81"/>
       <c r="BH4" s="81"/>
@@ -1567,227 +1570,227 @@
       <c r="G5" s="74"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>44858</v>
+        <v>44900</v>
       </c>
       <c r="J5" s="10">
         <f>I5+1</f>
-        <v>44859</v>
+        <v>44901</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
-        <v>44860</v>
+        <v>44902</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" si="0"/>
-        <v>44861</v>
+        <v>44903</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" si="0"/>
-        <v>44862</v>
+        <v>44904</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" si="0"/>
-        <v>44863</v>
+        <v>44905</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" si="0"/>
-        <v>44864</v>
+        <v>44906</v>
       </c>
       <c r="P5" s="11">
         <f>O5+1</f>
-        <v>44865</v>
+        <v>44907</v>
       </c>
       <c r="Q5" s="10">
         <f>P5+1</f>
-        <v>44866</v>
+        <v>44908</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" si="0"/>
-        <v>44867</v>
+        <v>44909</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" si="0"/>
-        <v>44868</v>
+        <v>44910</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" si="0"/>
-        <v>44869</v>
+        <v>44911</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" si="0"/>
-        <v>44870</v>
+        <v>44912</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" si="0"/>
-        <v>44871</v>
+        <v>44913</v>
       </c>
       <c r="W5" s="11">
         <f>V5+1</f>
-        <v>44872</v>
+        <v>44914</v>
       </c>
       <c r="X5" s="10">
         <f>W5+1</f>
-        <v>44873</v>
+        <v>44915</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" si="0"/>
-        <v>44874</v>
+        <v>44916</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" si="0"/>
-        <v>44875</v>
+        <v>44917</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" si="0"/>
-        <v>44876</v>
+        <v>44918</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" si="0"/>
-        <v>44877</v>
+        <v>44919</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" si="0"/>
-        <v>44878</v>
+        <v>44920</v>
       </c>
       <c r="AD5" s="11">
         <f>AC5+1</f>
-        <v>44879</v>
+        <v>44921</v>
       </c>
       <c r="AE5" s="10">
         <f>AD5+1</f>
-        <v>44880</v>
+        <v>44922</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" si="0"/>
-        <v>44881</v>
+        <v>44923</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" si="0"/>
-        <v>44882</v>
+        <v>44924</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" si="0"/>
-        <v>44883</v>
+        <v>44925</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" si="0"/>
-        <v>44884</v>
+        <v>44926</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" si="0"/>
-        <v>44885</v>
+        <v>44927</v>
       </c>
       <c r="AK5" s="11">
         <f>AJ5+1</f>
-        <v>44886</v>
+        <v>44928</v>
       </c>
       <c r="AL5" s="10">
         <f>AK5+1</f>
-        <v>44887</v>
+        <v>44929</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" si="0"/>
-        <v>44888</v>
+        <v>44930</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" si="0"/>
-        <v>44889</v>
+        <v>44931</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" si="0"/>
-        <v>44890</v>
+        <v>44932</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" si="0"/>
-        <v>44891</v>
+        <v>44933</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" si="0"/>
-        <v>44892</v>
+        <v>44934</v>
       </c>
       <c r="AR5" s="11">
         <f>AQ5+1</f>
-        <v>44893</v>
+        <v>44935</v>
       </c>
       <c r="AS5" s="10">
         <f>AR5+1</f>
-        <v>44894</v>
+        <v>44936</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" si="0"/>
-        <v>44895</v>
+        <v>44937</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" si="0"/>
-        <v>44896</v>
+        <v>44938</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" si="0"/>
-        <v>44897</v>
+        <v>44939</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" si="0"/>
-        <v>44898</v>
+        <v>44940</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" si="0"/>
-        <v>44899</v>
+        <v>44941</v>
       </c>
       <c r="AY5" s="11">
         <f>AX5+1</f>
-        <v>44900</v>
+        <v>44942</v>
       </c>
       <c r="AZ5" s="10">
         <f>AY5+1</f>
-        <v>44901</v>
+        <v>44943</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>44902</v>
+        <v>44944</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" si="1"/>
-        <v>44903</v>
+        <v>44945</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" si="1"/>
-        <v>44904</v>
+        <v>44946</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" si="1"/>
-        <v>44905</v>
+        <v>44947</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" si="1"/>
-        <v>44906</v>
+        <v>44948</v>
       </c>
       <c r="BF5" s="11">
         <f>BE5+1</f>
-        <v>44907</v>
+        <v>44949</v>
       </c>
       <c r="BG5" s="10">
         <f>BF5+1</f>
-        <v>44908</v>
+        <v>44950</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
-        <v>44909</v>
+        <v>44951</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" si="2"/>
-        <v>44910</v>
+        <v>44952</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" si="2"/>
-        <v>44911</v>
+        <v>44953</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" si="2"/>
-        <v>44912</v>
+        <v>44954</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" si="2"/>
-        <v>44913</v>
+        <v>44955</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1">
@@ -2118,7 +2121,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17" t="str">
-        <f t="shared" ref="H8:H37" ca="1" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H38" ca="1" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="44"/>
@@ -2753,13 +2756,13 @@
         <v>44856</v>
       </c>
       <c r="F16" s="56">
-        <f>E16+36</f>
-        <v>44892</v>
+        <f>E16+72</f>
+        <v>44928</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="I16" s="44"/>
       <c r="J16" s="44"/>
@@ -2827,7 +2830,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="27">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="E17" s="56">
         <f>E16</f>
@@ -2835,12 +2838,12 @@
       </c>
       <c r="F17" s="56">
         <f>F16</f>
-        <v>44892</v>
+        <v>44928</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="I17" s="44"/>
       <c r="J17" s="44"/>
@@ -2908,7 +2911,7 @@
         <v>27</v>
       </c>
       <c r="D18" s="27">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E18" s="56">
         <v>44883</v>
@@ -2988,7 +2991,7 @@
         <v>23</v>
       </c>
       <c r="D19" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="56">
         <f>F18</f>
@@ -3066,7 +3069,7 @@
         <v>27</v>
       </c>
       <c r="D20" s="27">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E20" s="56">
         <f>F18</f>
@@ -3225,7 +3228,7 @@
         <v>30</v>
       </c>
       <c r="D22" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="56">
         <v>44891</v>
@@ -3302,20 +3305,20 @@
         <v>25</v>
       </c>
       <c r="D23" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="56">
         <f>F22</f>
         <v>44895</v>
       </c>
       <c r="F23" s="56">
-        <f>E23+7</f>
-        <v>44902</v>
+        <f>E23+9</f>
+        <v>44904</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I23" s="44"/>
       <c r="J23" s="44"/>
@@ -3392,13 +3395,13 @@
         <v>44895</v>
       </c>
       <c r="F24" s="56">
-        <f>E24+7</f>
-        <v>44902</v>
+        <f t="shared" ref="F24:F27" si="7">E24+9</f>
+        <v>44904</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I24" s="44"/>
       <c r="J24" s="44"/>
@@ -3457,30 +3460,27 @@
       <c r="BK24" s="44"/>
       <c r="BL24" s="44"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A25" s="48"/>
       <c r="B25" s="70" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="63" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D25" s="27">
         <v>0</v>
       </c>
       <c r="E25" s="56">
-        <f>F22</f>
+        <f>F21</f>
         <v>44895</v>
       </c>
       <c r="F25" s="56">
-        <f>E25+7</f>
-        <v>44902</v>
+        <f t="shared" si="7"/>
+        <v>44904</v>
       </c>
       <c r="G25" s="17"/>
-      <c r="H25" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>8</v>
-      </c>
+      <c r="H25" s="17"/>
       <c r="I25" s="44"/>
       <c r="J25" s="44"/>
       <c r="K25" s="44"/>
@@ -3544,7 +3544,7 @@
         <v>44</v>
       </c>
       <c r="C26" s="63" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D26" s="27">
         <v>0</v>
@@ -3554,13 +3554,13 @@
         <v>44895</v>
       </c>
       <c r="F26" s="56">
-        <f>E26+7</f>
-        <v>44902</v>
+        <f t="shared" si="7"/>
+        <v>44904</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I26" s="44"/>
       <c r="J26" s="44"/>
@@ -3621,17 +3621,27 @@
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A27" s="48"/>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="64"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
+      <c r="C27" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="56">
+        <f>F22</f>
+        <v>44895</v>
+      </c>
+      <c r="F27" s="56">
+        <f t="shared" si="7"/>
+        <v>44904</v>
+      </c>
       <c r="G27" s="17"/>
-      <c r="H27" s="17" t="str">
+      <c r="H27" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="I27" s="44"/>
       <c r="J27" s="44"/>
@@ -3692,13 +3702,13 @@
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A28" s="48"/>
-      <c r="B28" s="71" t="s">
+      <c r="B28" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="65"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="31"/>
       <c r="G28" s="17"/>
       <c r="H28" s="17" t="str">
         <f t="shared" ca="1" si="6"/>
@@ -3833,9 +3843,7 @@
       <c r="BL29" s="44"/>
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A30" s="48" t="s">
-        <v>41</v>
-      </c>
+      <c r="A30" s="48"/>
       <c r="B30" s="71" t="s">
         <v>48</v>
       </c>
@@ -3906,7 +3914,9 @@
       <c r="BL30" s="44"/>
     </row>
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A31" s="48"/>
+      <c r="A31" s="48" t="s">
+        <v>41</v>
+      </c>
       <c r="B31" s="71" t="s">
         <v>49</v>
       </c>
@@ -4049,13 +4059,13 @@
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A33" s="48"/>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="66"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="36"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
       <c r="G33" s="17"/>
       <c r="H33" s="17" t="str">
         <f t="shared" ca="1" si="6"/>
@@ -4120,21 +4130,17 @@
     </row>
     <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A34" s="48"/>
-      <c r="B34" s="72" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="67"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="58" t="s">
+      <c r="B34" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="F34" s="58" t="s">
-        <v>52</v>
-      </c>
+      <c r="C34" s="66"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="17"/>
-      <c r="H34" s="17" t="e">
+      <c r="H34" s="17" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="I34" s="44"/>
       <c r="J34" s="44"/>
@@ -4201,10 +4207,10 @@
       <c r="C35" s="67"/>
       <c r="D35" s="37"/>
       <c r="E35" s="58" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F35" s="58" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G35" s="17"/>
       <c r="H35" s="17" t="e">
@@ -4269,19 +4275,17 @@
       <c r="BL35" s="44"/>
     </row>
     <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A36" s="48" t="s">
-        <v>53</v>
-      </c>
+      <c r="A36" s="48"/>
       <c r="B36" s="72" t="s">
         <v>48</v>
       </c>
       <c r="C36" s="67"/>
       <c r="D36" s="37"/>
       <c r="E36" s="58" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F36" s="58" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G36" s="17"/>
       <c r="H36" s="17" t="e">
@@ -4346,7 +4350,7 @@
       <c r="BL36" s="44"/>
     </row>
     <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="48" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="72" t="s">
@@ -4355,109 +4359,186 @@
       <c r="C37" s="67"/>
       <c r="D37" s="37"/>
       <c r="E37" s="58" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F37" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43" t="e">
+        <v>53</v>
+      </c>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17" t="e">
         <f t="shared" ca="1" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I37" s="46"/>
-      <c r="J37" s="46"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="46"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="46"/>
-      <c r="P37" s="46"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="46"/>
-      <c r="S37" s="46"/>
-      <c r="T37" s="46"/>
-      <c r="U37" s="46"/>
-      <c r="V37" s="46"/>
-      <c r="W37" s="46"/>
-      <c r="X37" s="46"/>
-      <c r="Y37" s="46"/>
-      <c r="Z37" s="46"/>
-      <c r="AA37" s="46"/>
-      <c r="AB37" s="46"/>
-      <c r="AC37" s="46"/>
-      <c r="AD37" s="46"/>
-      <c r="AE37" s="46"/>
-      <c r="AF37" s="46"/>
-      <c r="AG37" s="46"/>
-      <c r="AH37" s="46"/>
-      <c r="AI37" s="46"/>
-      <c r="AJ37" s="46"/>
-      <c r="AK37" s="46"/>
-      <c r="AL37" s="46"/>
-      <c r="AM37" s="46"/>
-      <c r="AN37" s="46"/>
-      <c r="AO37" s="46"/>
-      <c r="AP37" s="46"/>
-      <c r="AQ37" s="46"/>
-      <c r="AR37" s="46"/>
-      <c r="AS37" s="46"/>
-      <c r="AT37" s="46"/>
-      <c r="AU37" s="46"/>
-      <c r="AV37" s="46"/>
-      <c r="AW37" s="46"/>
-      <c r="AX37" s="46"/>
-      <c r="AY37" s="46"/>
-      <c r="AZ37" s="46"/>
-      <c r="BA37" s="46"/>
-      <c r="BB37" s="46"/>
-      <c r="BC37" s="46"/>
-      <c r="BD37" s="46"/>
-      <c r="BE37" s="46"/>
-      <c r="BF37" s="46"/>
-      <c r="BG37" s="46"/>
-      <c r="BH37" s="46"/>
-      <c r="BI37" s="46"/>
-      <c r="BJ37" s="46"/>
-      <c r="BK37" s="46"/>
-      <c r="BL37" s="46"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44"/>
+      <c r="N37" s="44"/>
+      <c r="O37" s="44"/>
+      <c r="P37" s="44"/>
+      <c r="Q37" s="44"/>
+      <c r="R37" s="44"/>
+      <c r="S37" s="44"/>
+      <c r="T37" s="44"/>
+      <c r="U37" s="44"/>
+      <c r="V37" s="44"/>
+      <c r="W37" s="44"/>
+      <c r="X37" s="44"/>
+      <c r="Y37" s="44"/>
+      <c r="Z37" s="44"/>
+      <c r="AA37" s="44"/>
+      <c r="AB37" s="44"/>
+      <c r="AC37" s="44"/>
+      <c r="AD37" s="44"/>
+      <c r="AE37" s="44"/>
+      <c r="AF37" s="44"/>
+      <c r="AG37" s="44"/>
+      <c r="AH37" s="44"/>
+      <c r="AI37" s="44"/>
+      <c r="AJ37" s="44"/>
+      <c r="AK37" s="44"/>
+      <c r="AL37" s="44"/>
+      <c r="AM37" s="44"/>
+      <c r="AN37" s="44"/>
+      <c r="AO37" s="44"/>
+      <c r="AP37" s="44"/>
+      <c r="AQ37" s="44"/>
+      <c r="AR37" s="44"/>
+      <c r="AS37" s="44"/>
+      <c r="AT37" s="44"/>
+      <c r="AU37" s="44"/>
+      <c r="AV37" s="44"/>
+      <c r="AW37" s="44"/>
+      <c r="AX37" s="44"/>
+      <c r="AY37" s="44"/>
+      <c r="AZ37" s="44"/>
+      <c r="BA37" s="44"/>
+      <c r="BB37" s="44"/>
+      <c r="BC37" s="44"/>
+      <c r="BD37" s="44"/>
+      <c r="BE37" s="44"/>
+      <c r="BF37" s="44"/>
+      <c r="BG37" s="44"/>
+      <c r="BH37" s="44"/>
+      <c r="BI37" s="44"/>
+      <c r="BJ37" s="44"/>
+      <c r="BK37" s="44"/>
+      <c r="BL37" s="44"/>
     </row>
-    <row r="38" spans="1:64" ht="30" customHeight="1">
+    <row r="38" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A38" s="49" t="s">
+        <v>55</v>
+      </c>
       <c r="B38" s="72" t="s">
         <v>50</v>
       </c>
       <c r="C38" s="67"/>
       <c r="D38" s="37"/>
       <c r="E38" s="58" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F38" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="G38" s="6"/>
+        <v>53</v>
+      </c>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
+      <c r="N38" s="46"/>
+      <c r="O38" s="46"/>
+      <c r="P38" s="46"/>
+      <c r="Q38" s="46"/>
+      <c r="R38" s="46"/>
+      <c r="S38" s="46"/>
+      <c r="T38" s="46"/>
+      <c r="U38" s="46"/>
+      <c r="V38" s="46"/>
+      <c r="W38" s="46"/>
+      <c r="X38" s="46"/>
+      <c r="Y38" s="46"/>
+      <c r="Z38" s="46"/>
+      <c r="AA38" s="46"/>
+      <c r="AB38" s="46"/>
+      <c r="AC38" s="46"/>
+      <c r="AD38" s="46"/>
+      <c r="AE38" s="46"/>
+      <c r="AF38" s="46"/>
+      <c r="AG38" s="46"/>
+      <c r="AH38" s="46"/>
+      <c r="AI38" s="46"/>
+      <c r="AJ38" s="46"/>
+      <c r="AK38" s="46"/>
+      <c r="AL38" s="46"/>
+      <c r="AM38" s="46"/>
+      <c r="AN38" s="46"/>
+      <c r="AO38" s="46"/>
+      <c r="AP38" s="46"/>
+      <c r="AQ38" s="46"/>
+      <c r="AR38" s="46"/>
+      <c r="AS38" s="46"/>
+      <c r="AT38" s="46"/>
+      <c r="AU38" s="46"/>
+      <c r="AV38" s="46"/>
+      <c r="AW38" s="46"/>
+      <c r="AX38" s="46"/>
+      <c r="AY38" s="46"/>
+      <c r="AZ38" s="46"/>
+      <c r="BA38" s="46"/>
+      <c r="BB38" s="46"/>
+      <c r="BC38" s="46"/>
+      <c r="BD38" s="46"/>
+      <c r="BE38" s="46"/>
+      <c r="BF38" s="46"/>
+      <c r="BG38" s="46"/>
+      <c r="BH38" s="46"/>
+      <c r="BI38" s="46"/>
+      <c r="BJ38" s="46"/>
+      <c r="BK38" s="46"/>
+      <c r="BL38" s="46"/>
     </row>
     <row r="39" spans="1:64" ht="30" customHeight="1">
-      <c r="B39" s="73"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="59"/>
-      <c r="F39" s="59"/>
+      <c r="B39" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="67"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:64" ht="30" customHeight="1">
-      <c r="B40" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" s="39"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="42"/>
+      <c r="B40" s="73"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="59"/>
     </row>
-    <row r="42" spans="1:64" ht="30" customHeight="1">
-      <c r="C42" s="14"/>
-      <c r="F42" s="50"/>
+    <row r="41" spans="1:64" ht="30" customHeight="1">
+      <c r="B41" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="39"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="42"/>
     </row>
     <row r="43" spans="1:64" ht="30" customHeight="1">
-      <c r="C43" s="15"/>
+      <c r="C43" s="14"/>
+      <c r="F43" s="50"/>
+    </row>
+    <row r="44" spans="1:64" ht="30" customHeight="1">
+      <c r="C44" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4473,7 +4554,7 @@
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D40">
+  <conditionalFormatting sqref="D7:D41">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4487,12 +4568,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL37">
+  <conditionalFormatting sqref="I5:BL38">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL37">
+  <conditionalFormatting sqref="I7:BL38">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4527,7 +4608,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D40</xm:sqref>
+          <xm:sqref>D7:D41</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>